<commit_message>
Disable 10% and free feature selection in RFE scripts
Commented out code related to 10% and free feature selection in both Bulbar_completo_rfe.py and Speech_test_loo.py, restricting analysis to the '5' feature selection technique. Updated results handling accordingly. Also moved and updated related Excel result files to the RFE/Swallowing subdirectories, removing old versions from the Results root.
</commit_message>
<xml_diff>
--- a/Results/RFE/Swallowing/MFCCs/swallowing_rfe.xlsx
+++ b/Results/RFE/Swallowing/MFCCs/swallowing_rfe.xlsx
@@ -506,7 +506,7 @@
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>Validation</t>
+          <t>F1 train</t>
         </is>
       </c>
     </row>
@@ -562,7 +562,7 @@
         <v>0.6666666666666666</v>
       </c>
       <c r="O2" t="n">
-        <v>0.8827106227106227</v>
+        <v>0.9411764705882353</v>
       </c>
     </row>
     <row r="3">
@@ -617,7 +617,7 @@
         <v>0.7777777777777778</v>
       </c>
       <c r="O3" t="n">
-        <v>0.7514652014652015</v>
+        <v>0.9565217391304348</v>
       </c>
     </row>
     <row r="4">
@@ -672,7 +672,7 @@
         <v>0.7777777777777778</v>
       </c>
       <c r="O4" t="n">
-        <v>0.823882783882784</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -727,7 +727,7 @@
         <v>0.6666666666666666</v>
       </c>
       <c r="O5" t="n">
-        <v>0.6605128205128205</v>
+        <v>0.7301587301587301</v>
       </c>
     </row>
     <row r="6">
@@ -782,7 +782,7 @@
         <v>0.4444444444444444</v>
       </c>
       <c r="O6" t="n">
-        <v>0.7104848093083387</v>
+        <v>0.7368421052631579</v>
       </c>
     </row>
     <row r="7">
@@ -892,7 +892,7 @@
         <v>0.6666666666666666</v>
       </c>
       <c r="O8" t="n">
-        <v>0.7967365967365969</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
@@ -947,7 +947,7 @@
         <v>0.6666666666666666</v>
       </c>
       <c r="O9" t="n">
-        <v>0.7958974358974359</v>
+        <v>0.9859154929577465</v>
       </c>
     </row>
     <row r="10">
@@ -1002,7 +1002,7 @@
         <v>0.5555555555555556</v>
       </c>
       <c r="O10" t="n">
-        <v>0.7372960372960373</v>
+        <v>0.9090909090909091</v>
       </c>
     </row>
     <row r="11">
@@ -1018,7 +1018,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>{'activation': 'tanh', 'alpha': 0.0001, 'hidden_layer_sizes': (32, 16), 'learning_rate': 'constant'}</t>
+          <t>{'activation': 'tanh', 'alpha': 0.0001, 'hidden_layer_sizes': (64, 32), 'learning_rate': 'constant'}</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1027,37 +1027,37 @@
         </is>
       </c>
       <c r="E11" t="n">
+        <v>3</v>
+      </c>
+      <c r="F11" t="n">
+        <v>3</v>
+      </c>
+      <c r="G11" t="n">
+        <v>8</v>
+      </c>
+      <c r="H11" t="n">
         <v>6</v>
       </c>
-      <c r="F11" t="n">
-        <v>2</v>
-      </c>
-      <c r="G11" t="n">
-        <v>9</v>
-      </c>
-      <c r="H11" t="n">
-        <v>3</v>
-      </c>
       <c r="I11" t="n">
-        <v>0.75</v>
+        <v>0.55</v>
       </c>
       <c r="J11" t="n">
-        <v>0.7058823529411765</v>
+        <v>0.4</v>
       </c>
       <c r="K11" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="L11" t="n">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="M11" t="n">
-        <v>0.8181818181818182</v>
+        <v>0.7272727272727273</v>
       </c>
       <c r="N11" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="O11" t="n">
-        <v>0.6318266253869969</v>
+        <v>0.9117647058823529</v>
       </c>
     </row>
     <row r="12">
@@ -1112,7 +1112,7 @@
         <v>0.6666666666666666</v>
       </c>
       <c r="O12" t="n">
-        <v>0.9179487179487179</v>
+        <v>0.8333333333333334</v>
       </c>
     </row>
     <row r="13">
@@ -1167,7 +1167,7 @@
         <v>0.6666666666666666</v>
       </c>
       <c r="O13" t="n">
-        <v>0.8145604395604396</v>
+        <v>0.8857142857142857</v>
       </c>
     </row>
     <row r="14">
@@ -1222,7 +1222,7 @@
         <v>0.6666666666666666</v>
       </c>
       <c r="O14" t="n">
-        <v>0.8002530802530803</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15">
@@ -1277,7 +1277,7 @@
         <v>0.7777777777777778</v>
       </c>
       <c r="O15" t="n">
-        <v>0.8052813852813852</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
@@ -1332,7 +1332,7 @@
         <v>0.7777777777777778</v>
       </c>
       <c r="O16" t="n">
-        <v>0.7200653594771242</v>
+        <v>0.6590909090909091</v>
       </c>
     </row>
   </sheetData>

</xml_diff>